<commit_message>
Finish grading of lab08
</commit_message>
<xml_diff>
--- a/lab/lab8/lab08_Section1.xlsx
+++ b/lab/lab8/lab08_Section1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liumanni/Documents/CSE 220/cse220_2020fall/lab/lab8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5419592E-E5EE-1D4D-92EF-CB031DDC519D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAE58D4-2DA5-7A4C-9C10-CC2DFA62479F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{1C3543F5-1004-B644-A376-BBD6DC1ED258}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Huynh, Tommy</t>
-  </si>
-  <si>
-    <t>Jeurink, Sydney</t>
   </si>
   <si>
     <t>Jirjees, Rani</t>
@@ -504,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C37B7-F0BE-684B-BEEA-5AEE1918F2D1}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="106" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="106" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,9 +633,12 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -646,11 +646,8 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>17</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -662,6 +659,9 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -731,14 +731,14 @@
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -764,17 +764,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A18" r:id="rId1" tooltip="Compose email to Connor Kempisty" display="javascript://" xr:uid="{46E85C0E-175C-E547-9D29-E72A7AFF7F92}"/>
+    <hyperlink ref="A17" r:id="rId1" tooltip="Compose email to Connor Kempisty" display="javascript://" xr:uid="{46E85C0E-175C-E547-9D29-E72A7AFF7F92}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>